<commit_message>
updated throughput graphs with rescent results
</commit_message>
<xml_diff>
--- a/tests/graphs/compare.xlsx
+++ b/tests/graphs/compare.xlsx
@@ -12,7 +12,8 @@
     <sheet name="Latency (All)" sheetId="10" r:id="rId3"/>
     <sheet name="TP (All)" sheetId="12" r:id="rId4"/>
     <sheet name="TP (get,del)" sheetId="13" r:id="rId5"/>
-    <sheet name="Sheet2" sheetId="15" r:id="rId6"/>
+    <sheet name="TP (put)" sheetId="16" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="15" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Table!$B$2:$I$2</definedName>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="25">
   <si>
     <t>k</t>
   </si>
@@ -95,14 +96,16 @@
   <si>
     <t>t</t>
   </si>
+  <si>
+    <t>del</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
-    <numFmt numFmtId="165" formatCode="0.0000000000000"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -755,7 +758,6 @@
   </cellStyleXfs>
   <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -783,15 +785,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="42" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -812,6 +805,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -931,9 +934,27 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:multiLvlStrRef>
+            <c:strRef>
               <c:f>Table!$E$13:$E$17</c:f>
-            </c:multiLvlStrRef>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1+1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32+516</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64+1024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96+1540</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128+2048</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -979,9 +1000,27 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:multiLvlStrRef>
+            <c:strRef>
               <c:f>Table!$E$13:$E$17</c:f>
-            </c:multiLvlStrRef>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1+1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32+516</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64+1024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96+1540</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128+2048</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1019,11 +1058,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="68004480"/>
-        <c:axId val="78316288"/>
+        <c:axId val="71744512"/>
+        <c:axId val="190107648"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="68004480"/>
+        <c:axId val="71744512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1051,7 +1090,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78316288"/>
+        <c:crossAx val="190107648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1059,7 +1098,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78316288"/>
+        <c:axId val="190107648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3.180000000000001E-3"/>
@@ -1097,7 +1136,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68004480"/>
+        <c:crossAx val="71744512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1172,9 +1211,27 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:multiLvlStrRef>
+            <c:strRef>
               <c:f>Table!$E$13:$E$17</c:f>
-            </c:multiLvlStrRef>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1+1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32+516</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64+1024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96+1540</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128+2048</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1220,9 +1277,27 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:multiLvlStrRef>
+            <c:strRef>
               <c:f>Table!$E$13:$E$17</c:f>
-            </c:multiLvlStrRef>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1+1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32+516</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64+1024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96+1540</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128+2048</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1268,9 +1343,27 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:multiLvlStrRef>
+            <c:strRef>
               <c:f>Table!$E$13:$E$17</c:f>
-            </c:multiLvlStrRef>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1+1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32+516</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64+1024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96+1540</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128+2048</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1308,11 +1401,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="40770560"/>
-        <c:axId val="40776832"/>
+        <c:axId val="190127488"/>
+        <c:axId val="190133760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="40770560"/>
+        <c:axId val="190127488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1345,7 +1438,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40776832"/>
+        <c:crossAx val="190133760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1353,7 +1446,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40776832"/>
+        <c:axId val="190133760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.21000000000000002"/>
@@ -1385,7 +1478,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40770560"/>
+        <c:crossAx val="190127488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1460,9 +1553,27 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:multiLvlStrRef>
+            <c:strRef>
               <c:f>Table!$E$13:$E$17</c:f>
-            </c:multiLvlStrRef>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1+1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32+516</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64+1024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96+1540</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128+2048</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1471,19 +1582,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>111.48043379110837</c:v>
+                  <c:v>1785.9617781223756</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>107.27575783644781</c:v>
+                  <c:v>1616.5819843779745</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>102.35741396817937</c:v>
+                  <c:v>1349.2982826447767</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>175.06086461390612</c:v>
+                  <c:v>1211.7284588829784</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>110.73093488227829</c:v>
+                  <c:v>1084.5144710869727</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1508,9 +1619,27 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:multiLvlStrRef>
+            <c:strRef>
               <c:f>Table!$E$13:$E$17</c:f>
-            </c:multiLvlStrRef>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1+1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32+516</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64+1024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96+1540</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128+2048</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1519,19 +1648,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>113.720743135489</c:v>
+                  <c:v>1646.3792154553348</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>101.67601144252957</c:v>
+                  <c:v>1585.4030718013025</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>92.871383574730714</c:v>
+                  <c:v>1519.9471354763443</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>91.789376058962546</c:v>
+                  <c:v>1325.484865870108</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>98.630272021844476</c:v>
+                  <c:v>1162.6749620668563</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1556,9 +1685,27 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:multiLvlStrRef>
+            <c:strRef>
               <c:f>Table!$E$13:$E$17</c:f>
-            </c:multiLvlStrRef>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1+1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32+516</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64+1024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96+1540</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128+2048</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1567,19 +1714,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5.4461698102144691</c:v>
+                  <c:v>6.1280143068787885</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0160823629674374</c:v>
+                  <c:v>5.5903482670434306</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.9194675295131551</c:v>
+                  <c:v>5.6608548030657939</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.5205874215574626</c:v>
+                  <c:v>5.3991750535427467</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.7613764773784286</c:v>
+                  <c:v>5.1667906262056924</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1596,11 +1743,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="189539072"/>
-        <c:axId val="189540992"/>
+        <c:axId val="191316736"/>
+        <c:axId val="191318656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="189539072"/>
+        <c:axId val="191316736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1633,7 +1780,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="189540992"/>
+        <c:crossAx val="191318656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1641,10 +1788,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189540992"/>
+        <c:axId val="191318656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="200"/>
+          <c:max val="1800"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1673,7 +1820,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="189539072"/>
+        <c:crossAx val="191316736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1748,9 +1895,27 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:multiLvlStrRef>
+            <c:strRef>
               <c:f>Table!$E$13:$E$17</c:f>
-            </c:multiLvlStrRef>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1+1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32+516</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64+1024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96+1540</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128+2048</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1759,19 +1924,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>111.48043379110837</c:v>
+                  <c:v>1785.9617781223756</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>107.27575783644781</c:v>
+                  <c:v>1616.5819843779745</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>102.35741396817937</c:v>
+                  <c:v>1349.2982826447767</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>175.06086461390612</c:v>
+                  <c:v>1211.7284588829784</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>110.73093488227829</c:v>
+                  <c:v>1084.5144710869727</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1796,9 +1961,27 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:multiLvlStrRef>
+            <c:strRef>
               <c:f>Table!$E$13:$E$17</c:f>
-            </c:multiLvlStrRef>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1+1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32+516</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64+1024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96+1540</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128+2048</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1807,19 +1990,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>113.720743135489</c:v>
+                  <c:v>1646.3792154553348</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>101.67601144252957</c:v>
+                  <c:v>1585.4030718013025</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>92.871383574730714</c:v>
+                  <c:v>1519.9471354763443</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>91.789376058962546</c:v>
+                  <c:v>1325.484865870108</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>98.630272021844476</c:v>
+                  <c:v>1162.6749620668563</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1836,11 +2019,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="189560320"/>
-        <c:axId val="189562240"/>
+        <c:axId val="191351808"/>
+        <c:axId val="191431808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="189560320"/>
+        <c:axId val="191351808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1873,7 +2056,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="189562240"/>
+        <c:crossAx val="191431808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1881,10 +2064,220 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189562240"/>
+        <c:axId val="191431808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="200"/>
+          <c:max val="1800"/>
+          <c:min val="1000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Operations per second</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="191351808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Throughput</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Table!$A$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Put</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Table!$E$13:$E$17</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1+1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32+516</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64+1024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96+1540</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128+2048</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Table!$G$31:$G$35</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>6.1280143068787885</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.5903482670434306</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.6608548030657939</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.3991750535427467</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.1667906262056924</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="191446016"/>
+        <c:axId val="191497344"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="191446016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Key Size</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> + Value Size</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="191497344"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="191497344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="8"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1913,7 +2306,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="189560320"/>
+        <c:crossAx val="191446016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1965,6 +2358,17 @@
 </file>
 
 <file path=xl/chartsheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
@@ -2057,6 +2461,33 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8667750" cy="6296025"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -2370,859 +2801,1595 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P35"/>
+  <dimension ref="A1:X35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="4" width="9.140625" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="2" max="5" width="9.140625" customWidth="1"/>
     <col min="6" max="9" width="14.140625" customWidth="1"/>
-    <col min="13" max="16" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="12" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
+    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K1" s="27">
+        <v>1</v>
+      </c>
+      <c r="L1">
+        <v>1</v>
+      </c>
+      <c r="M1">
+        <v>1.23489189148</v>
+      </c>
+      <c r="P1">
+        <v>1</v>
+      </c>
+      <c r="Q1">
+        <v>1</v>
+      </c>
+      <c r="R1">
+        <v>1.12300300598</v>
+      </c>
+      <c r="U1">
+        <v>1</v>
+      </c>
+      <c r="V1">
+        <v>1</v>
+      </c>
+      <c r="W1">
+        <v>149.87958502800001</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="K2" s="27">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1.22067594528</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1.10986804962</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <v>152.453923941</v>
+      </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>1</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>1</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>2</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="7">
         <v>1.2227E-2</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="7">
         <v>2.2750000000000001E-3</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="7">
         <v>2.7999962500000015E-3</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="7">
         <v>4.9597973236843338E-4</v>
       </c>
+      <c r="K3" s="27">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1.2145490646399999</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1.14511013031</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3">
+        <v>153.90131402</v>
+      </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="29"/>
+      <c r="B4" s="2">
         <v>32</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>516</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>548</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>5.8250000000000003E-3</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <v>2.2590000000000002E-3</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="4">
         <v>2.8738862499999977E-3</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="4">
         <v>3.9960649914295163E-4</v>
       </c>
+      <c r="K4" s="27">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1.1968839168500001</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>1.10139799118</v>
+      </c>
+      <c r="S4">
+        <f>AVERAGE(R1:R4)</f>
+        <v>1.1198447942725001</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4">
+        <v>1</v>
+      </c>
+      <c r="W4">
+        <v>155.15781903300001</v>
+      </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="29"/>
+      <c r="B5" s="2">
         <v>64</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>1024</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>1088</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>9.2149999999999992E-3</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>2.2780000000000001E-3</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="4">
         <v>3.057358525921297E-3</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="4">
         <v>4.8060943356204104E-4</v>
       </c>
+      <c r="K5" s="27">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1.2069339752199999</v>
+      </c>
+      <c r="N5">
+        <f>AVERAGE(M1:M5)</f>
+        <v>1.2147869586940001</v>
+      </c>
+      <c r="P5">
+        <v>32</v>
+      </c>
+      <c r="Q5">
+        <v>516</v>
+      </c>
+      <c r="R5">
+        <v>1.1656668186200001</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5">
+        <v>1</v>
+      </c>
+      <c r="W5">
+        <v>204.53234601</v>
+      </c>
+      <c r="X5">
+        <f>AVERAGE(W1:W5)</f>
+        <v>163.1849976064</v>
+      </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" s="29"/>
+      <c r="B6" s="2">
         <v>96</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>1540</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>1636</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>1.0004000000000001E-2</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>2.3839999999999998E-3</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="4">
         <v>3.0939100000000014E-3</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="4">
         <v>4.6608919356730963E-4</v>
       </c>
+      <c r="K6" s="27">
+        <v>32</v>
+      </c>
+      <c r="L6">
+        <v>516</v>
+      </c>
+      <c r="M6">
+        <v>1.2484049797100001</v>
+      </c>
+      <c r="P6">
+        <v>32</v>
+      </c>
+      <c r="Q6">
+        <v>516</v>
+      </c>
+      <c r="R6">
+        <v>1.2750549316399999</v>
+      </c>
+      <c r="U6">
+        <v>32</v>
+      </c>
+      <c r="V6">
+        <v>516</v>
+      </c>
+      <c r="W6">
+        <v>171.88433599499999</v>
+      </c>
     </row>
-    <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="19"/>
-      <c r="B7" s="4">
+    <row r="7" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="30"/>
+      <c r="B7" s="3">
         <v>128</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>2048</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>2176</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>8.6809999999999995E-3</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <v>2.2850000000000001E-3</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <v>3.1671262500000013E-3</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="5">
         <v>5.9590843747348878E-4</v>
       </c>
+      <c r="K7" s="27">
+        <v>32</v>
+      </c>
+      <c r="L7">
+        <v>516</v>
+      </c>
+      <c r="M7">
+        <v>1.2535061836200001</v>
+      </c>
+      <c r="P7">
+        <v>32</v>
+      </c>
+      <c r="Q7">
+        <v>516</v>
+      </c>
+      <c r="R7">
+        <v>1.3525049686399999</v>
+      </c>
+      <c r="U7">
+        <v>32</v>
+      </c>
+      <c r="V7">
+        <v>516</v>
+      </c>
+      <c r="W7">
+        <v>174.47902107199999</v>
+      </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>1</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <v>1</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="6">
         <v>2</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="7">
         <v>5.8310000000000002E-3</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="7">
         <v>2.3050000000000002E-3</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="7">
         <v>3.0061712500000001E-3</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="7">
         <v>4.3005053230538794E-4</v>
       </c>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
+      <c r="K8" s="27">
+        <v>32</v>
+      </c>
+      <c r="L8">
+        <v>516</v>
+      </c>
+      <c r="M8">
+        <v>1.2904300689699999</v>
+      </c>
+      <c r="P8">
+        <v>32</v>
+      </c>
+      <c r="Q8">
+        <v>516</v>
+      </c>
+      <c r="R8">
+        <v>1.15548610687</v>
+      </c>
+      <c r="S8">
+        <f>AVERAGE(R5:R8)</f>
+        <v>1.2371782064424999</v>
+      </c>
+      <c r="U8">
+        <v>32</v>
+      </c>
+      <c r="V8">
+        <v>516</v>
+      </c>
+      <c r="W8">
+        <v>174.70630598100001</v>
+      </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" s="29"/>
+      <c r="B9" s="2">
         <v>32</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>516</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>548</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>6.476E-3</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="4">
         <v>2.2889999999999998E-3</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="4">
         <v>2.7444318750000003E-3</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="4">
         <v>3.5702742643037798E-4</v>
       </c>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
+      <c r="K9" s="27">
+        <v>32</v>
+      </c>
+      <c r="L9">
+        <v>516</v>
+      </c>
+      <c r="M9">
+        <v>1.2431640625</v>
+      </c>
+      <c r="P9">
+        <v>64</v>
+      </c>
+      <c r="Q9">
+        <v>1024</v>
+      </c>
+      <c r="R9">
+        <v>1.3296279907199999</v>
+      </c>
+      <c r="U9">
+        <v>32</v>
+      </c>
+      <c r="V9">
+        <v>516</v>
+      </c>
+      <c r="W9">
+        <v>176.94029212000001</v>
+      </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" s="29"/>
+      <c r="B10" s="2">
         <v>64</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>1024</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>1088</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>7.5799999999999999E-3</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <v>2.2539999999999999E-3</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="4">
         <v>2.9437932542161135E-3</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="4">
         <v>3.8998757076920534E-4</v>
       </c>
+      <c r="K10" s="27">
+        <v>32</v>
+      </c>
+      <c r="L10">
+        <v>516</v>
+      </c>
+      <c r="M10">
+        <v>1.27203893661</v>
+      </c>
+      <c r="N10">
+        <f>AVERAGE(M6:M10)</f>
+        <v>1.2615088462820001</v>
+      </c>
+      <c r="P10">
+        <v>64</v>
+      </c>
+      <c r="Q10">
+        <v>1024</v>
+      </c>
+      <c r="R10">
+        <v>1.5132598877000001</v>
+      </c>
+      <c r="U10">
+        <v>32</v>
+      </c>
+      <c r="V10">
+        <v>516</v>
+      </c>
+      <c r="W10">
+        <v>196.388705015</v>
+      </c>
+      <c r="X10">
+        <f>AVERAGE(W6:W10)</f>
+        <v>178.87973203659999</v>
+      </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11" s="29"/>
+      <c r="B11" s="2">
         <v>96</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>1540</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>1636</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>5.2919999999999998E-3</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="4">
         <v>2.343E-3</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="4">
         <v>3.0542406250000037E-3</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="4">
         <v>3.6946522748570001E-4</v>
       </c>
+      <c r="K11" s="27">
+        <v>64</v>
+      </c>
+      <c r="L11">
+        <v>1024</v>
+      </c>
+      <c r="M11">
+        <v>1.33045315742</v>
+      </c>
+      <c r="P11">
+        <v>64</v>
+      </c>
+      <c r="Q11">
+        <v>1024</v>
+      </c>
+      <c r="R11">
+        <v>1.5626318454699999</v>
+      </c>
+      <c r="U11">
+        <v>64</v>
+      </c>
+      <c r="V11">
+        <v>1024</v>
+      </c>
+      <c r="W11">
+        <v>171.877707958</v>
+      </c>
     </row>
-    <row r="12" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19"/>
-      <c r="B12" s="4">
+    <row r="12" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="30"/>
+      <c r="B12" s="3">
         <v>128</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>2048</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>2176</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="5">
         <v>5.5040000000000002E-3</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="5">
         <v>2.3410000000000002E-3</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="5">
         <v>3.0147625000000035E-3</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="5">
         <v>4.3903861494136405E-4</v>
       </c>
+      <c r="K12" s="27">
+        <v>64</v>
+      </c>
+      <c r="L12">
+        <v>1024</v>
+      </c>
+      <c r="M12">
+        <v>1.31989192963</v>
+      </c>
+      <c r="P12">
+        <v>64</v>
+      </c>
+      <c r="Q12">
+        <v>1024</v>
+      </c>
+      <c r="R12">
+        <v>1.5234880447400001</v>
+      </c>
+      <c r="S12">
+        <f>AVERAGE(R9:R12)</f>
+        <v>1.4822519421575002</v>
+      </c>
+      <c r="U12">
+        <v>64</v>
+      </c>
+      <c r="V12">
+        <v>1024</v>
+      </c>
+      <c r="W12">
+        <v>177.99538588499999</v>
+      </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>1</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <v>1</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="6">
         <v>2</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="7">
         <v>0.475717</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="7">
         <v>0.12525500000000001</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="7">
         <v>0.17647565874999988</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="7">
         <v>5.0957266697786725E-2</v>
       </c>
+      <c r="K13" s="27">
+        <v>64</v>
+      </c>
+      <c r="L13">
+        <v>1024</v>
+      </c>
+      <c r="M13">
+        <v>1.28122901917</v>
+      </c>
+      <c r="P13">
+        <v>96</v>
+      </c>
+      <c r="Q13">
+        <v>1540</v>
+      </c>
+      <c r="R13">
+        <v>1.5226860046399999</v>
+      </c>
+      <c r="U13">
+        <v>64</v>
+      </c>
+      <c r="V13">
+        <v>1024</v>
+      </c>
+      <c r="W13">
+        <v>177.70504617700001</v>
+      </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14" s="29"/>
+      <c r="B14" s="2">
         <v>32</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>516</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>548</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="4">
         <v>0.445905</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="4">
         <v>0.13275400000000001</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14" s="4">
         <v>0.18885591124999984</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I14" s="4">
         <v>5.8704388257428179E-2</v>
       </c>
+      <c r="K14" s="27">
+        <v>64</v>
+      </c>
+      <c r="L14">
+        <v>1024</v>
+      </c>
+      <c r="M14">
+        <v>1.29649496078</v>
+      </c>
+      <c r="P14">
+        <v>96</v>
+      </c>
+      <c r="Q14">
+        <v>1540</v>
+      </c>
+      <c r="R14">
+        <v>1.7053580284100001</v>
+      </c>
+      <c r="U14">
+        <v>64</v>
+      </c>
+      <c r="V14">
+        <v>1024</v>
+      </c>
+      <c r="W14">
+        <v>178.22853684399999</v>
+      </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A15" s="29"/>
+      <c r="B15" s="2">
         <v>64</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>1024</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
         <v>1088</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="4">
         <v>0.47451399999999999</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="4">
         <v>0.132882</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H15" s="4">
         <v>0.19264039600249824</v>
       </c>
-      <c r="I15" s="5">
+      <c r="I15" s="4">
         <v>6.3034157312142722E-2</v>
       </c>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
+      <c r="K15" s="27">
+        <v>64</v>
+      </c>
+      <c r="L15">
+        <v>1024</v>
+      </c>
+      <c r="M15">
+        <v>1.35110712051</v>
+      </c>
+      <c r="N15">
+        <f>AVERAGE(M11:M15)</f>
+        <v>1.3158352375019999</v>
+      </c>
+      <c r="P15">
+        <v>96</v>
+      </c>
+      <c r="Q15">
+        <v>1540</v>
+      </c>
+      <c r="R15">
+        <v>1.64191508293</v>
+      </c>
+      <c r="U15">
+        <v>64</v>
+      </c>
+      <c r="V15">
+        <v>1024</v>
+      </c>
+      <c r="W15">
+        <v>177.45215487499999</v>
+      </c>
+      <c r="X15">
+        <f>AVERAGE(W11:W15)</f>
+        <v>176.65176634779999</v>
+      </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A16" s="29"/>
+      <c r="B16" s="2">
         <v>96</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <v>1540</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="2">
         <v>1636</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="4">
         <v>0.55771199999999999</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="4">
         <v>0.13245399999999999</v>
       </c>
-      <c r="H16" s="5">
+      <c r="H16" s="4">
         <v>0.19735985375000017</v>
       </c>
-      <c r="I16" s="5">
+      <c r="I16" s="4">
         <v>6.1433795957953299E-2</v>
       </c>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
+      <c r="K16" s="27">
+        <v>96</v>
+      </c>
+      <c r="L16">
+        <v>1540</v>
+      </c>
+      <c r="M16">
+        <v>1.51501584053</v>
+      </c>
+      <c r="P16">
+        <v>96</v>
+      </c>
+      <c r="Q16">
+        <v>1540</v>
+      </c>
+      <c r="R16">
+        <v>1.7321801185600001</v>
+      </c>
+      <c r="S16">
+        <f>AVERAGE(R13:R16)</f>
+        <v>1.6505348086349998</v>
+      </c>
+      <c r="U16">
+        <v>96</v>
+      </c>
+      <c r="V16">
+        <v>1540</v>
+      </c>
+      <c r="W16">
+        <v>178.51047611199999</v>
+      </c>
     </row>
-    <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="19"/>
-      <c r="B17" s="4">
+    <row r="17" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="30"/>
+      <c r="B17" s="3">
         <v>128</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <v>2048</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <v>2176</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="5">
         <v>0.424369</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="5">
         <v>0.13234599999999999</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H17" s="5">
         <v>0.1970279081250004</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I17" s="5">
         <v>6.011823934827068E-2</v>
       </c>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
+      <c r="K17" s="27">
+        <v>96</v>
+      </c>
+      <c r="L17">
+        <v>1540</v>
+      </c>
+      <c r="M17">
+        <v>1.50972795486</v>
+      </c>
+      <c r="P17">
+        <v>128</v>
+      </c>
+      <c r="Q17">
+        <v>2048</v>
+      </c>
+      <c r="R17">
+        <v>1.75486803055</v>
+      </c>
+      <c r="U17">
+        <v>96</v>
+      </c>
+      <c r="V17">
+        <v>1540</v>
+      </c>
+      <c r="W17">
+        <v>201.03612113</v>
+      </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E18" s="15"/>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="E18" s="14"/>
+      <c r="K18" s="27">
+        <v>96</v>
+      </c>
+      <c r="L18">
+        <v>1540</v>
+      </c>
+      <c r="M18">
+        <v>1.4789459705400001</v>
+      </c>
+      <c r="P18">
+        <v>128</v>
+      </c>
+      <c r="Q18">
+        <v>2048</v>
+      </c>
+      <c r="R18">
+        <v>1.88873791695</v>
+      </c>
+      <c r="U18">
+        <v>96</v>
+      </c>
+      <c r="V18">
+        <v>1540</v>
+      </c>
+      <c r="W18">
+        <v>180.909692049</v>
+      </c>
     </row>
-    <row r="19" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E19" s="15"/>
+    <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E19" s="14"/>
+      <c r="K19" s="27">
+        <v>96</v>
+      </c>
+      <c r="L19">
+        <v>1540</v>
+      </c>
+      <c r="M19">
+        <v>1.53040313721</v>
+      </c>
+      <c r="P19">
+        <v>128</v>
+      </c>
+      <c r="Q19">
+        <v>2048</v>
+      </c>
+      <c r="R19">
+        <v>1.8141348362</v>
+      </c>
+      <c r="U19">
+        <v>96</v>
+      </c>
+      <c r="V19">
+        <v>1540</v>
+      </c>
+      <c r="W19">
+        <v>181.80978083599999</v>
+      </c>
     </row>
-    <row r="20" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="2" t="s">
+    <row r="20" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="H20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K20" s="27">
+        <v>96</v>
+      </c>
+      <c r="L20">
+        <v>1540</v>
+      </c>
+      <c r="M20">
+        <v>1.5103161334999999</v>
+      </c>
+      <c r="N20">
+        <f>AVERAGE(M16:M20)</f>
+        <v>1.5088818073279999</v>
+      </c>
+      <c r="P20">
+        <v>128</v>
+      </c>
+      <c r="Q20">
+        <v>2048</v>
+      </c>
+      <c r="R20">
+        <v>1.91883206367</v>
+      </c>
+      <c r="S20">
+        <f>AVERAGE(R17:R20)</f>
+        <v>1.8441432118425001</v>
+      </c>
+      <c r="U20">
+        <v>96</v>
+      </c>
+      <c r="V20">
+        <v>1540</v>
+      </c>
+      <c r="W20">
+        <v>183.80132913599999</v>
+      </c>
+      <c r="X20">
+        <f>AVERAGE(W16:W20)</f>
+        <v>185.21347985259999</v>
+      </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A21" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="6">
         <v>1</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="6">
         <v>1</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="6">
         <v>2</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E21" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F21" s="7">
+        <f>S4</f>
+        <v>1.1198447942725001</v>
+      </c>
+      <c r="G21" s="8">
+        <f>2000/F21</f>
+        <v>1785.9617781223756</v>
+      </c>
+      <c r="H21" s="7">
         <v>17.9403679371</v>
       </c>
-      <c r="G21" s="9">
-        <f>2000/F21</f>
-        <v>111.48043379110837</v>
+      <c r="K21" s="27">
+        <v>128</v>
+      </c>
+      <c r="L21">
+        <v>2048</v>
+      </c>
+      <c r="M21">
+        <v>1.7464230060599999</v>
+      </c>
+      <c r="P21" t="s">
+        <v>18</v>
+      </c>
+      <c r="U21">
+        <v>128</v>
+      </c>
+      <c r="V21">
+        <v>2048</v>
+      </c>
+      <c r="W21">
+        <v>177.43073582599999</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" s="3">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A22" s="29"/>
+      <c r="B22" s="2">
         <v>32</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <v>516</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="2">
         <v>548</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F22" s="4">
+        <f>S8</f>
+        <v>1.2371782064424999</v>
+      </c>
+      <c r="G22" s="9">
+        <f t="shared" ref="G22:G30" si="0">2000/F22</f>
+        <v>1616.5819843779745</v>
+      </c>
+      <c r="H22" s="4">
         <v>18.6435410976</v>
       </c>
-      <c r="G22" s="10">
-        <f t="shared" ref="G22:G35" si="0">2000/F22</f>
-        <v>107.27575783644781</v>
+      <c r="K22" s="27">
+        <v>128</v>
+      </c>
+      <c r="L22">
+        <v>2048</v>
+      </c>
+      <c r="M22">
+        <v>1.70203113556</v>
+      </c>
+      <c r="U22">
+        <v>128</v>
+      </c>
+      <c r="V22">
+        <v>2048</v>
+      </c>
+      <c r="W22">
+        <v>227.287566185</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-      <c r="B23" s="3">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A23" s="29"/>
+      <c r="B23" s="2">
         <v>64</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <v>1024</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="2">
         <v>1088</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E23" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F23" s="4">
+        <f>S12</f>
+        <v>1.4822519421575002</v>
+      </c>
+      <c r="G23" s="9">
+        <f t="shared" si="0"/>
+        <v>1349.2982826447767</v>
+      </c>
+      <c r="H23" s="4">
         <v>19.539376020399999</v>
       </c>
-      <c r="G23" s="10">
+      <c r="K23" s="27">
+        <v>128</v>
+      </c>
+      <c r="L23">
+        <v>2048</v>
+      </c>
+      <c r="M23">
+        <v>1.7381339073199999</v>
+      </c>
+      <c r="U23">
+        <v>128</v>
+      </c>
+      <c r="V23">
+        <v>2048</v>
+      </c>
+      <c r="W23">
+        <v>183.69420003900001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A24" s="29"/>
+      <c r="B24" s="2">
+        <v>96</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1540</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1636</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="4">
+        <f>S16</f>
+        <v>1.6505348086349998</v>
+      </c>
+      <c r="G24" s="9">
         <f t="shared" si="0"/>
-        <v>102.35741396817937</v>
+        <v>1211.7284588829784</v>
+      </c>
+      <c r="H24" s="4">
+        <v>11.4245979786</v>
+      </c>
+      <c r="K24" s="27">
+        <v>128</v>
+      </c>
+      <c r="L24">
+        <v>2048</v>
+      </c>
+      <c r="M24">
+        <v>1.6812889576000001</v>
+      </c>
+      <c r="U24">
+        <v>128</v>
+      </c>
+      <c r="V24">
+        <v>2048</v>
+      </c>
+      <c r="W24">
+        <v>194.80804491000001</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
-      <c r="B24" s="3">
+    <row r="25" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="30"/>
+      <c r="B25" s="3">
+        <v>128</v>
+      </c>
+      <c r="C25" s="3">
+        <v>2048</v>
+      </c>
+      <c r="D25" s="3">
+        <v>2176</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="5">
+        <f>S20</f>
+        <v>1.8441432118425001</v>
+      </c>
+      <c r="G25" s="10">
+        <f t="shared" si="0"/>
+        <v>1084.5144710869727</v>
+      </c>
+      <c r="H25" s="5">
+        <v>18.0618000031</v>
+      </c>
+      <c r="K25" s="27">
+        <v>128</v>
+      </c>
+      <c r="L25">
+        <v>2048</v>
+      </c>
+      <c r="M25">
+        <v>1.7329790592200001</v>
+      </c>
+      <c r="N25">
+        <f>AVERAGE(M21:M25)</f>
+        <v>1.7201712131520002</v>
+      </c>
+      <c r="U25">
+        <v>128</v>
+      </c>
+      <c r="V25">
+        <v>2048</v>
+      </c>
+      <c r="W25">
+        <v>184.498170853</v>
+      </c>
+      <c r="X25">
+        <f>AVERAGE(W21:W25)</f>
+        <v>193.54374356260001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A26" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="6">
+        <v>1</v>
+      </c>
+      <c r="C26" s="6">
+        <v>1</v>
+      </c>
+      <c r="D26" s="6">
+        <v>2</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="7">
+        <f>N5</f>
+        <v>1.2147869586940001</v>
+      </c>
+      <c r="G26" s="8">
+        <f t="shared" si="0"/>
+        <v>1646.3792154553348</v>
+      </c>
+      <c r="H26" s="7">
+        <v>17.586940999999999</v>
+      </c>
+      <c r="I26" s="7"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A27" s="29"/>
+      <c r="B27" s="2">
+        <v>32</v>
+      </c>
+      <c r="C27" s="2">
+        <v>516</v>
+      </c>
+      <c r="D27" s="2">
+        <v>548</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="4">
+        <f>N10</f>
+        <v>1.2615088462820001</v>
+      </c>
+      <c r="G27" s="9">
+        <f t="shared" si="0"/>
+        <v>1585.4030718013025</v>
+      </c>
+      <c r="H27" s="4">
+        <v>19.670323133499998</v>
+      </c>
+      <c r="I27" s="4"/>
+      <c r="K27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A28" s="29"/>
+      <c r="B28" s="2">
+        <v>64</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1024</v>
+      </c>
+      <c r="D28" s="2">
+        <v>1088</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="4">
+        <f>N15</f>
+        <v>1.3158352375019999</v>
+      </c>
+      <c r="G28" s="9">
+        <f t="shared" si="0"/>
+        <v>1519.9471354763443</v>
+      </c>
+      <c r="H28" s="4">
+        <v>21.5351588726</v>
+      </c>
+      <c r="I28" s="4"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A29" s="29"/>
+      <c r="B29" s="2">
         <v>96</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C29" s="2">
         <v>1540</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D29" s="2">
         <v>1636</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="E29" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F24" s="5">
-        <v>11.4245979786</v>
-      </c>
-      <c r="G24" s="10">
+      <c r="F29" s="4">
+        <f>N20</f>
+        <v>1.5088818073279999</v>
+      </c>
+      <c r="G29" s="9">
         <f t="shared" si="0"/>
-        <v>175.06086461390612</v>
-      </c>
+        <v>1325.484865870108</v>
+      </c>
+      <c r="H29" s="4">
+        <v>21.789014000000002</v>
+      </c>
+      <c r="I29" s="4"/>
     </row>
-    <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="19"/>
-      <c r="B25" s="4">
+    <row r="30" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="30"/>
+      <c r="B30" s="3">
         <v>128</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C30" s="3">
         <v>2048</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D30" s="3">
         <v>2176</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E30" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F25" s="6">
-        <v>18.0618000031</v>
-      </c>
-      <c r="G25" s="11">
+      <c r="F30" s="5">
+        <f>N25</f>
+        <v>1.7201712131520002</v>
+      </c>
+      <c r="G30" s="10">
         <f t="shared" si="0"/>
-        <v>110.73093488227829</v>
-      </c>
+        <v>1162.6749620668563</v>
+      </c>
+      <c r="H30" s="5">
+        <v>20.277750015300001</v>
+      </c>
+      <c r="I30" s="5"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B26" s="7">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A31" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="6">
         <v>1</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C31" s="6">
         <v>1</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D31" s="6">
         <v>2</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="E31" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F26" s="8">
-        <v>17.586940999999999</v>
-      </c>
-      <c r="G26" s="9">
-        <f t="shared" si="0"/>
-        <v>113.720743135489</v>
-      </c>
-      <c r="I26" s="8">
-        <v>29.636515140499998</v>
+      <c r="F31" s="7">
+        <f>X5</f>
+        <v>163.1849976064</v>
+      </c>
+      <c r="G31" s="8">
+        <f>1000/F31</f>
+        <v>6.1280143068787885</v>
+      </c>
+      <c r="H31" s="7">
+        <v>367.23056197199998</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
-      <c r="B27" s="3">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A32" s="29"/>
+      <c r="B32" s="2">
         <v>32</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C32" s="2">
         <v>516</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D32" s="2">
         <v>548</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="E32" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F27" s="5">
-        <v>19.670323133499998</v>
-      </c>
-      <c r="G27" s="10">
-        <f t="shared" si="0"/>
-        <v>101.67601144252957</v>
-      </c>
-      <c r="I27" s="5">
-        <v>19.670323133499998</v>
+      <c r="F32" s="4">
+        <f>X10</f>
+        <v>178.87973203659999</v>
+      </c>
+      <c r="G32" s="9">
+        <f t="shared" ref="G32:G35" si="1">1000/F32</f>
+        <v>5.5903482670434306</v>
+      </c>
+      <c r="H32" s="4">
+        <v>398.717535973</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
-      <c r="B28" s="3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="29"/>
+      <c r="B33" s="2">
         <v>64</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C33" s="2">
         <v>1024</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D33" s="2">
         <v>1088</v>
       </c>
-      <c r="E28" s="13" t="s">
+      <c r="E33" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F28" s="5">
-        <v>21.5351588726</v>
-      </c>
-      <c r="G28" s="10">
-        <f t="shared" si="0"/>
-        <v>92.871383574730714</v>
-      </c>
-      <c r="I28" s="5">
-        <v>21.5351588726</v>
+      <c r="F33" s="4">
+        <f>X15</f>
+        <v>176.65176634779999</v>
+      </c>
+      <c r="G33" s="9">
+        <f t="shared" si="1"/>
+        <v>5.6608548030657939</v>
+      </c>
+      <c r="H33" s="4">
+        <v>406.54806399300003</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
-      <c r="B29" s="3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="29"/>
+      <c r="B34" s="2">
         <v>96</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C34" s="2">
         <v>1540</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D34" s="2">
         <v>1636</v>
       </c>
-      <c r="E29" s="13" t="s">
+      <c r="E34" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F29" s="5">
-        <v>21.789014000000002</v>
-      </c>
-      <c r="G29" s="10">
-        <f t="shared" si="0"/>
-        <v>91.789376058962546</v>
-      </c>
-      <c r="I29" s="5">
-        <v>1.4799599647499999</v>
+      <c r="F34" s="4">
+        <f>X20</f>
+        <v>185.21347985259999</v>
+      </c>
+      <c r="G34" s="9">
+        <f t="shared" si="1"/>
+        <v>5.3991750535427467</v>
+      </c>
+      <c r="H34" s="4">
+        <v>442.42037892299999</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="19"/>
-      <c r="B30" s="4">
+    <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="30"/>
+      <c r="B35" s="3">
         <v>128</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C35" s="3">
         <v>2048</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D35" s="3">
         <v>2176</v>
       </c>
-      <c r="E30" s="14" t="s">
+      <c r="E35" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F30" s="6">
-        <v>20.277750015300001</v>
-      </c>
-      <c r="G30" s="11">
-        <f t="shared" si="0"/>
-        <v>98.630272021844476</v>
-      </c>
-      <c r="I30" s="6">
-        <v>20.277750015300001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B31" s="7">
-        <v>1</v>
-      </c>
-      <c r="C31" s="7">
-        <v>1</v>
-      </c>
-      <c r="D31" s="7">
-        <v>2</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="F31" s="8">
-        <v>367.23056197199998</v>
-      </c>
-      <c r="G31" s="9">
-        <f t="shared" si="0"/>
-        <v>5.4461698102144691</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
-      <c r="B32" s="3">
-        <v>32</v>
-      </c>
-      <c r="C32" s="3">
-        <v>516</v>
-      </c>
-      <c r="D32" s="3">
-        <v>548</v>
-      </c>
-      <c r="E32" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F32" s="5">
-        <v>398.717535973</v>
-      </c>
-      <c r="G32" s="10">
-        <f t="shared" si="0"/>
-        <v>5.0160823629674374</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
-      <c r="B33" s="3">
-        <v>64</v>
-      </c>
-      <c r="C33" s="3">
-        <v>1024</v>
-      </c>
-      <c r="D33" s="3">
-        <v>1088</v>
-      </c>
-      <c r="E33" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F33" s="5">
-        <v>406.54806399300003</v>
-      </c>
-      <c r="G33" s="10">
-        <f t="shared" si="0"/>
-        <v>4.9194675295131551</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
-      <c r="B34" s="3">
-        <v>96</v>
-      </c>
-      <c r="C34" s="3">
-        <v>1540</v>
-      </c>
-      <c r="D34" s="3">
-        <v>1636</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F34" s="5">
-        <v>442.42037892299999</v>
-      </c>
-      <c r="G34" s="10">
-        <f t="shared" si="0"/>
-        <v>4.5205874215574626</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="19"/>
-      <c r="B35" s="4">
-        <v>128</v>
-      </c>
-      <c r="C35" s="4">
-        <v>2048</v>
-      </c>
-      <c r="D35" s="4">
-        <v>2176</v>
-      </c>
-      <c r="E35" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F35" s="6">
+      <c r="F35" s="5">
+        <f>X25</f>
+        <v>193.54374356260001</v>
+      </c>
+      <c r="G35" s="10">
+        <f t="shared" si="1"/>
+        <v>5.1667906262056924</v>
+      </c>
+      <c r="H35" s="5">
         <v>420.04659986500002</v>
-      </c>
-      <c r="G35" s="11">
-        <f t="shared" si="0"/>
-        <v>4.7613764773784286</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B2:J26">
-    <sortCondition ref="B2:B26"/>
-    <sortCondition ref="C2:C26"/>
+  <sortState ref="U1:W35">
+    <sortCondition ref="U1:U35"/>
   </sortState>
   <mergeCells count="6">
     <mergeCell ref="A31:A35"/>
@@ -3233,6 +4400,46 @@
     <mergeCell ref="A26:A30"/>
   </mergeCells>
   <conditionalFormatting sqref="I14">
+    <cfRule type="colorScale" priority="80">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H14">
+    <cfRule type="colorScale" priority="79">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G14">
+    <cfRule type="colorScale" priority="78">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F14">
+    <cfRule type="colorScale" priority="77">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14">
     <cfRule type="colorScale" priority="76">
       <colorScale>
         <cfvo type="min"/>
@@ -3242,7 +4449,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H14">
+  <conditionalFormatting sqref="C14">
     <cfRule type="colorScale" priority="75">
       <colorScale>
         <cfvo type="min"/>
@@ -3252,7 +4459,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G14">
+  <conditionalFormatting sqref="D14">
     <cfRule type="colorScale" priority="74">
       <colorScale>
         <cfvo type="min"/>
@@ -3262,7 +4469,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F14">
+  <conditionalFormatting sqref="I13">
     <cfRule type="colorScale" priority="73">
       <colorScale>
         <cfvo type="min"/>
@@ -3272,7 +4479,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14">
+  <conditionalFormatting sqref="H13">
     <cfRule type="colorScale" priority="72">
       <colorScale>
         <cfvo type="min"/>
@@ -3282,7 +4489,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
+  <conditionalFormatting sqref="G13">
     <cfRule type="colorScale" priority="71">
       <colorScale>
         <cfvo type="min"/>
@@ -3292,7 +4499,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
+  <conditionalFormatting sqref="F13">
     <cfRule type="colorScale" priority="70">
       <colorScale>
         <cfvo type="min"/>
@@ -3302,7 +4509,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
+  <conditionalFormatting sqref="B13">
     <cfRule type="colorScale" priority="69">
       <colorScale>
         <cfvo type="min"/>
@@ -3312,7 +4519,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H13">
+  <conditionalFormatting sqref="C13">
     <cfRule type="colorScale" priority="68">
       <colorScale>
         <cfvo type="min"/>
@@ -3322,7 +4529,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G13">
+  <conditionalFormatting sqref="D13">
     <cfRule type="colorScale" priority="67">
       <colorScale>
         <cfvo type="min"/>
@@ -3332,7 +4539,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F13">
+  <conditionalFormatting sqref="I12">
     <cfRule type="colorScale" priority="66">
       <colorScale>
         <cfvo type="min"/>
@@ -3342,7 +4549,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B13">
+  <conditionalFormatting sqref="H12">
     <cfRule type="colorScale" priority="65">
       <colorScale>
         <cfvo type="min"/>
@@ -3352,7 +4559,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13">
+  <conditionalFormatting sqref="G12">
     <cfRule type="colorScale" priority="64">
       <colorScale>
         <cfvo type="min"/>
@@ -3362,7 +4569,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13">
+  <conditionalFormatting sqref="F12">
     <cfRule type="colorScale" priority="63">
       <colorScale>
         <cfvo type="min"/>
@@ -3372,7 +4579,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I12">
+  <conditionalFormatting sqref="B12">
     <cfRule type="colorScale" priority="62">
       <colorScale>
         <cfvo type="min"/>
@@ -3382,7 +4589,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H12">
+  <conditionalFormatting sqref="C12">
     <cfRule type="colorScale" priority="61">
       <colorScale>
         <cfvo type="min"/>
@@ -3392,7 +4599,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G12">
+  <conditionalFormatting sqref="D12">
     <cfRule type="colorScale" priority="60">
       <colorScale>
         <cfvo type="min"/>
@@ -3402,7 +4609,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F12">
+  <conditionalFormatting sqref="B8:B17">
     <cfRule type="colorScale" priority="59">
       <colorScale>
         <cfvo type="min"/>
@@ -3412,7 +4619,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B12">
+  <conditionalFormatting sqref="C8:C17">
     <cfRule type="colorScale" priority="58">
       <colorScale>
         <cfvo type="min"/>
@@ -3422,7 +4629,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C12">
+  <conditionalFormatting sqref="D8:D17">
     <cfRule type="colorScale" priority="57">
       <colorScale>
         <cfvo type="min"/>
@@ -3432,7 +4639,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D12">
+  <conditionalFormatting sqref="F3:F17">
     <cfRule type="colorScale" priority="56">
       <colorScale>
         <cfvo type="min"/>
@@ -3442,7 +4649,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B8:B17">
+  <conditionalFormatting sqref="G1:G19 G36:G1048576">
     <cfRule type="colorScale" priority="55">
       <colorScale>
         <cfvo type="min"/>
@@ -3452,7 +4659,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:C17">
+  <conditionalFormatting sqref="H1:H19 H36:H1048576">
     <cfRule type="colorScale" priority="54">
       <colorScale>
         <cfvo type="min"/>
@@ -3462,7 +4669,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D17">
+  <conditionalFormatting sqref="I1:I25 I31:I1048576">
     <cfRule type="colorScale" priority="53">
       <colorScale>
         <cfvo type="min"/>
@@ -3472,37 +4679,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F17">
-    <cfRule type="colorScale" priority="52">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEF9C"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G19 G36:G1048576">
-    <cfRule type="colorScale" priority="51">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEF9C"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="colorScale" priority="50">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEF9C"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I1:I25 I31:I1048576">
+  <conditionalFormatting sqref="G32">
     <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min"/>
@@ -3512,7 +4689,37 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G32">
+  <conditionalFormatting sqref="F32">
+    <cfRule type="colorScale" priority="48">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32">
+    <cfRule type="colorScale" priority="47">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32">
+    <cfRule type="colorScale" priority="46">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32">
     <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
@@ -3522,7 +4729,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F32">
+  <conditionalFormatting sqref="G31">
     <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min"/>
@@ -3532,7 +4739,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B32">
+  <conditionalFormatting sqref="F31">
     <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>
@@ -3542,7 +4749,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C32">
+  <conditionalFormatting sqref="B31">
     <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
@@ -3552,7 +4759,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D32">
+  <conditionalFormatting sqref="C31">
     <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
@@ -3562,7 +4769,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G31">
+  <conditionalFormatting sqref="D31">
     <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
@@ -3572,7 +4779,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F31">
+  <conditionalFormatting sqref="G30">
     <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
@@ -3582,7 +4789,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B31">
+  <conditionalFormatting sqref="F30">
     <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min"/>
@@ -3592,7 +4799,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C31">
+  <conditionalFormatting sqref="B30">
     <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
@@ -3602,7 +4809,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D31">
+  <conditionalFormatting sqref="C30">
     <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
@@ -3612,7 +4819,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G30">
+  <conditionalFormatting sqref="D30">
     <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
@@ -3622,7 +4829,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F30">
+  <conditionalFormatting sqref="B26:B35">
     <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
@@ -3632,7 +4839,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B30">
+  <conditionalFormatting sqref="C26:C35">
     <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
@@ -3642,7 +4849,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C30">
+  <conditionalFormatting sqref="D26:D35">
     <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
@@ -3652,7 +4859,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D30">
+  <conditionalFormatting sqref="F21:F35">
     <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
@@ -3662,7 +4869,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B26:B35">
+  <conditionalFormatting sqref="G20:G35">
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
@@ -3672,7 +4879,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C26:C35">
+  <conditionalFormatting sqref="B7">
     <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
@@ -3682,7 +4889,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D26:D35">
+  <conditionalFormatting sqref="C7">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
@@ -3692,7 +4899,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F21:F35">
+  <conditionalFormatting sqref="D7:E7">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -3702,7 +4909,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G20:G35">
+  <conditionalFormatting sqref="B3:B7">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
@@ -3712,7 +4919,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7">
+  <conditionalFormatting sqref="C3:C7">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
@@ -3722,7 +4929,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7">
+  <conditionalFormatting sqref="D3:E7">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
@@ -3732,7 +4939,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D7:E7">
+  <conditionalFormatting sqref="B25">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -3742,7 +4949,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B7">
+  <conditionalFormatting sqref="C25">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -3752,7 +4959,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C7">
+  <conditionalFormatting sqref="D25">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -3762,7 +4969,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:E7">
+  <conditionalFormatting sqref="B21:B25">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -3772,7 +4979,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B25">
+  <conditionalFormatting sqref="C21:C25">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -3782,7 +4989,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C25">
+  <conditionalFormatting sqref="D21:D25">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -3792,17 +4999,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D25">
+  <conditionalFormatting sqref="G21:G35">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEF9C"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B21:B25">
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -3812,7 +5019,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21:C25">
+  <conditionalFormatting sqref="E8:E12">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -3822,7 +5029,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D21:D25">
+  <conditionalFormatting sqref="E17">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -3832,17 +5039,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G21:G35">
+  <conditionalFormatting sqref="E13:E17">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E12">
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -3852,7 +5059,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E8:E12">
+  <conditionalFormatting sqref="E21:E25">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -3862,7 +5069,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E17">
+  <conditionalFormatting sqref="E30">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -3872,7 +5079,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E13:E17">
+  <conditionalFormatting sqref="E26:E30">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -3882,7 +5089,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
+  <conditionalFormatting sqref="E35">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -3892,7 +5099,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E21:E25">
+  <conditionalFormatting sqref="E31:E35">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -3902,7 +5109,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E30">
+  <conditionalFormatting sqref="I30">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -3912,7 +5119,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E26:E30">
+  <conditionalFormatting sqref="I26:I30">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -3922,7 +5129,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E35">
+  <conditionalFormatting sqref="H32">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -3932,7 +5139,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E31:E35">
+  <conditionalFormatting sqref="H31">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -3942,7 +5149,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I30">
+  <conditionalFormatting sqref="H30">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -3952,7 +5159,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I26:I30">
+  <conditionalFormatting sqref="H21:H35">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -4001,257 +5208,257 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="21">
+      <c r="B2" s="17">
         <v>2000</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="17">
         <v>1</v>
       </c>
-      <c r="D2" s="21">
+      <c r="D2" s="17">
         <v>1</v>
       </c>
-      <c r="E2" s="22">
+      <c r="E2" s="18">
         <v>29.636515140499998</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="20">
         <v>2000</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C3" s="20">
         <v>32</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="20">
         <v>516</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="21">
         <v>19.670323133499998</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="20">
         <v>2000</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="20">
         <v>64</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="20">
         <v>1024</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="21">
         <v>21.5351588726</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="20">
         <v>2000</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="20">
         <v>96</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="20">
         <v>1540</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="21">
         <v>1.4799599647499999</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B6" s="24">
         <v>2000</v>
       </c>
-      <c r="C6" s="28">
+      <c r="C6" s="24">
         <v>128</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D6" s="24">
         <v>2048</v>
       </c>
-      <c r="E6" s="29">
+      <c r="E6" s="25">
         <v>20.277750015300001</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="17">
         <v>2000</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="17">
         <v>1</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="17">
         <v>1</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="18">
         <v>17.9403679371</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="24">
+      <c r="B8" s="20">
         <v>2000</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="20">
         <v>32</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="20">
         <v>516</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="21">
         <v>18.6435410976</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="24">
+      <c r="B9" s="20">
         <v>2000</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="20">
         <v>64</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="20">
         <v>1024</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="21">
         <v>19.539376020399999</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="24">
+      <c r="B10" s="20">
         <v>2000</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="20">
         <v>96</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="20">
         <v>1540</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="21">
         <v>11.4245979786</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="28">
+      <c r="B11" s="24">
         <v>2000</v>
       </c>
-      <c r="C11" s="28">
+      <c r="C11" s="24">
         <v>128</v>
       </c>
-      <c r="D11" s="28">
+      <c r="D11" s="24">
         <v>2048</v>
       </c>
-      <c r="E11" s="29">
+      <c r="E11" s="25">
         <v>18.0618000031</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12" s="17">
         <v>2000</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="17">
         <v>1</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="17">
         <v>1</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="18">
         <v>367.23056197199998</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="24">
+      <c r="B13" s="20">
         <v>2000</v>
       </c>
-      <c r="C13" s="24">
+      <c r="C13" s="20">
         <v>32</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13" s="20">
         <v>516</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="21">
         <v>398.717535973</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="24">
+      <c r="B14" s="20">
         <v>2000</v>
       </c>
-      <c r="C14" s="24">
+      <c r="C14" s="20">
         <v>64</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="20">
         <v>1024</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="21">
         <v>406.54806399300003</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="24">
+      <c r="B15" s="20">
         <v>2000</v>
       </c>
-      <c r="C15" s="24">
+      <c r="C15" s="20">
         <v>96</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D15" s="20">
         <v>1540</v>
       </c>
-      <c r="E15" s="25">
+      <c r="E15" s="21">
         <v>442.42037892299999</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="28">
+      <c r="B16" s="24">
         <v>2000</v>
       </c>
-      <c r="C16" s="28">
+      <c r="C16" s="24">
         <v>128</v>
       </c>
-      <c r="D16" s="28">
+      <c r="D16" s="24">
         <v>2048</v>
       </c>
-      <c r="E16" s="29">
+      <c r="E16" s="25">
         <v>420.04659986500002</v>
       </c>
     </row>

</xml_diff>